<commit_message>
after contact test case
</commit_message>
<xml_diff>
--- a/7RmartSupermarket/src/test/resources/TestData.xlsx
+++ b/7RmartSupermarket/src/test/resources/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\git\7RMartSupermarketProject\7RmartSupermarket\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE79D8A-0A14-46ED-B359-B39A766E75FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCCFD85-540B-4AA2-91A4-103C52A0FC31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{39C9072A-21C4-4A05-87CC-696BDB291405}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>username</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Rs.10/km</t>
+  </si>
+  <si>
+    <t>+917788445511</t>
   </si>
 </sst>
 </file>
@@ -184,13 +187,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,12 +688,12 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
@@ -697,7 +701,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B1" t="s">
@@ -714,8 +718,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>7788445511</v>
+      <c r="A2" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
@@ -735,5 +739,8 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{03AEB92C-303E-4400-BE25-3CD55E16659C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>